<commit_message>
Enhance ExcelSheetManager with workbook and sheet integrity checks: Implement async method to ensure workbook and sheets exist, optionally filling with mock data. Update integrity check in TestExcelPage to reflect new functionality and improve error handling. Add test data population feature in test-excel-products script for easier testing.
</commit_message>
<xml_diff>
--- a/tmp/TestBillingData.xlsx
+++ b/tmp/TestBillingData.xlsx
@@ -400,52 +400,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="D1" t="str">
+        <v>category</v>
+      </c>
+      <c r="E1" t="str">
+        <v>price</v>
+      </c>
+      <c r="F1" t="str">
+        <v>cost_price</v>
+      </c>
+      <c r="G1" t="str">
+        <v>stock_quantity</v>
+      </c>
+      <c r="H1" t="str">
+        <v>unit</v>
+      </c>
+      <c r="I1" t="str">
+        <v>hsn_code</v>
+      </c>
+      <c r="J1" t="str">
+        <v>gst_rate</v>
+      </c>
+      <c r="K1" t="str">
+        <v>is_active</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>594e2ff5-1dac-4141-bfbf-0888c697862a</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Alpha Widget</v>
+      </c>
+      <c r="C2" t="str">
+        <v>AW-100</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Widgets</v>
+      </c>
+      <c r="E2">
+        <v>99.99</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2" t="str">
+        <v>piece</v>
+      </c>
+      <c r="I2" t="str">
+        <v>1001</v>
+      </c>
+      <c r="J2">
+        <v>18</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>d6647f0d-be66-49c0-9947-304d0d13eaad</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Beta Gadget</v>
+      </c>
+      <c r="C3" t="str">
+        <v>BG-200</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Gadgets</v>
+      </c>
+      <c r="E3">
+        <v>149.5</v>
+      </c>
+      <c r="F3">
+        <v>120</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="str">
+        <v>piece</v>
+      </c>
+      <c r="I3" t="str">
+        <v>2002</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="E1" t="str">
+        <v>gstin</v>
+      </c>
+      <c r="F1" t="str">
+        <v>address</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>b4059366-584f-45d1-b842-2e2054e9b7f1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C2" t="str">
+        <v>john@example.com</v>
+      </c>
+      <c r="D2" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v>123 Road City</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>38269074-e958-4faf-bd21-474a68066b72</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Acme Corp</v>
+      </c>
+      <c r="C3" t="str">
+        <v>acme@corp.com</v>
+      </c>
+      <c r="D3" t="str">
+        <v>5550002222</v>
+      </c>
+      <c r="E3" t="str">
+        <v>27AACCA1234F1Z2</v>
+      </c>
+      <c r="F3" t="str">
+        <v>456 Industrial Area</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>title</v>
+      </c>
+      <c r="D1" t="str">
+        <v>salary</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>92653c1f-0553-4d9a-a9d9-6d5942787f97</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Jane Smith</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Manager</v>
+      </c>
+      <c r="D2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>8e8d9d86-43b8-421b-87ba-1a743b5d61ca</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Bob Miller</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Staff</v>
+      </c>
+      <c r="D3">
+        <v>30000</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>customer_id</v>
+      </c>
+      <c r="C1" t="str">
+        <v>total</v>
+      </c>
+      <c r="D1" t="str">
+        <v>created_at</v>
+      </c>
+      <c r="E1" t="str">
+        <v>items</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>c6443c74-26d6-4a65-b20f-20ad1e015232</v>
+      </c>
+      <c r="B2" t="str">
+        <v>b4059366-584f-45d1-b842-2e2054e9b7f1</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-10-30T14:54:07.153Z</v>
+      </c>
+      <c r="E2" t="str">
+        <v>[{"product_id":"594e2ff5-1dac-4141-bfbf-0888c697862a","qty":2,"price":99.99}]</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>5ecf3b24-9c3a-4e8c-9b99-aede363b2077</v>
+      </c>
+      <c r="B3" t="str">
+        <v>38269074-e958-4faf-bd21-474a68066b72</v>
+      </c>
+      <c r="C3">
+        <v>149.5</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-10-30T14:54:07.154Z</v>
+      </c>
+      <c r="E3" t="str">
+        <v>[{"product_id":"d6647f0d-be66-49c0-9947-304d0d13eaad","qty":1,"price":149.5}]</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>